<commit_message>
Fixed the peer_range pic, added quite a bit to the importance of epsilon
</commit_message>
<xml_diff>
--- a/experiments/Excel Charts/eps1.0,budg=eps,peers5-55,groups5,reg2e2-data500-pubAll-adult-groupbypeerverification-3-testsetmeanPeerRangeTest.xlsx
+++ b/experiments/Excel Charts/eps1.0,budg=eps,peers5-55,groups5,reg2e2-data500-pubAll-adult-groupbypeerverification-3-testsetmeanPeerRangeTest.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter\Documents\MML\mml-2015\experiments\Excel Charts\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="135" windowWidth="21075" windowHeight="10560"/>
   </bookViews>
@@ -11,10 +16,6 @@
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -550,6 +551,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -557,7 +561,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="nn-NO"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -758,11 +762,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="47199872"/>
-        <c:axId val="47200448"/>
+        <c:axId val="186336688"/>
+        <c:axId val="186337248"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="47199872"/>
+        <c:axId val="186336688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="50"/>
@@ -774,13 +778,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="47200448"/>
+        <c:crossAx val="186337248"/>
         <c:crossesAt val="1.0000000000000004E-6"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="47200448"/>
+        <c:axId val="186337248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.70000000000000007"/>
@@ -793,7 +797,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="47199872"/>
+        <c:crossAx val="186336688"/>
         <c:crossesAt val="1.0000000000000004E-6"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
@@ -949,7 +953,7 @@
               <a:latin typeface="+mn-lt"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>aggregatednd and local model</a:t>
+            <a:t>aggregated and local model</a:t>
           </a:r>
         </a:p>
       </cdr:txBody>
@@ -1113,7 +1117,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1148,7 +1152,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1640,7 +1644,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
       <selection sqref="A1:B10"/>
     </sheetView>
   </sheetViews>

</xml_diff>